<commit_message>
create script for analysis, add missing 1991 event in present block
</commit_message>
<xml_diff>
--- a/documents/participants_info.xlsx
+++ b/documents/participants_info.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="69">
   <si>
     <t>Participant</t>
   </si>
@@ -201,6 +201,36 @@
   </si>
   <si>
     <t>25/04/19 à 16h06</t>
+  </si>
+  <si>
+    <t>Mme Guitton</t>
+  </si>
+  <si>
+    <t>charlotte.guitton2496@orange.fr</t>
+  </si>
+  <si>
+    <t>caro.couteret@laposte.net</t>
+  </si>
+  <si>
+    <t>Mme Couteret</t>
+  </si>
+  <si>
+    <t>30/04/19 à 14h46</t>
+  </si>
+  <si>
+    <t>07/05/19 de 16h00 à 17h30</t>
+  </si>
+  <si>
+    <t>expérience passée 3 fois</t>
+  </si>
+  <si>
+    <t>expérience passée 2 fois</t>
+  </si>
+  <si>
+    <t>expérience passée 2 fois (+1 fois où pygame a crashé)</t>
+  </si>
+  <si>
+    <t>30/04/19 à 14h51</t>
   </si>
 </sst>
 </file>
@@ -250,7 +280,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -265,6 +295,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -549,13 +582,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="10" width="35.77734375" customWidth="1"/>
+    <col min="1" max="1" width="35.77734375" customWidth="1"/>
+    <col min="2" max="2" width="15.77734375" customWidth="1"/>
+    <col min="3" max="10" width="35.77734375" customWidth="1"/>
     <col min="11" max="11" width="100.77734375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -613,11 +648,15 @@
       <c r="F2" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G2" s="1"/>
+      <c r="G2" s="6">
+        <v>0.92</v>
+      </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
+      <c r="K2" s="1" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="3" spans="1:11" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -690,11 +729,15 @@
       <c r="F5" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G5" s="1"/>
+      <c r="G5" s="6">
+        <v>0.76</v>
+      </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
+      <c r="K5" s="1" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="6" spans="1:11" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
@@ -765,23 +808,35 @@
       <c r="F8" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="G8" s="1"/>
+      <c r="G8" s="6">
+        <v>1</v>
+      </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
+      <c r="K8" s="1" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="9" spans="1:11" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="1"/>
+      <c r="A9" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="B9" s="1">
         <v>8</v>
       </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
+      <c r="C9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>60</v>
+      </c>
       <c r="E9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="1"/>
+      <c r="F9" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
@@ -789,16 +844,24 @@
       <c r="K9" s="1"/>
     </row>
     <row r="10" spans="1:11" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="1"/>
+      <c r="A10" s="1" t="s">
+        <v>62</v>
+      </c>
       <c r="B10" s="1">
         <v>9</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
+      <c r="C10" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>61</v>
+      </c>
       <c r="E10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F10" s="1"/>
+      <c r="F10" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>

</xml_diff>

<commit_message>
separate participant analysis and general analysis in two scripts
</commit_message>
<xml_diff>
--- a/documents/participants_info.xlsx
+++ b/documents/participants_info.xlsx
@@ -635,8 +635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C3" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="E9" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -952,7 +952,9 @@
       <c r="F11" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="G11" s="1"/>
+      <c r="G11" s="6">
+        <v>1</v>
+      </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>

</xml_diff>